<commit_message>
Module language usage added.
</commit_message>
<xml_diff>
--- a/.Archive/Modules.xlsx
+++ b/.Archive/Modules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\just4\OneDrive\MSc Advanced Computer Science\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\just4\OneDrive\ACS\.Archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{E37F52FD-022F-497B-93C7-3FDF21401B11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{58EF10B1-070A-477A-B8D2-4C0128BE6E00}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{E37F52FD-022F-497B-93C7-3FDF21401B11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FB9541B9-A7AA-4250-B85C-8953E28B8E9D}"/>
   <bookViews>
     <workbookView xWindow="498" yWindow="-96" windowWidth="22638" windowHeight="13152" xr2:uid="{FD200E5E-48CC-4B06-828A-E1CDBAD2990E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Evaluation Methods and Statistics</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>2h lectures + 4h lab</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Jupyter</t>
+  </si>
+  <si>
+    <t>Java</t>
   </si>
 </sst>
 </file>
@@ -171,13 +180,13 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC33294-859F-476B-B46D-0E8F900EE8B6}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -507,7 +516,7 @@
     <col min="5" max="9" width="10.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -525,7 +534,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,8 +553,11 @@
       <c r="F2" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -564,8 +576,11 @@
       <c r="F3" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -584,8 +599,11 @@
       <c r="F4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -604,22 +622,25 @@
       <c r="F5" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -639,7 +660,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -659,7 +680,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -672,14 +693,14 @@
       <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5" t="s">
+      <c r="E9" s="2">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -687,7 +708,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -695,8 +716,8 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1"/>
@@ -705,7 +726,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -717,7 +738,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -729,7 +750,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -741,7 +762,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:7" ht="20.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>